<commit_message>
Added 4 Planning Area of Residences data (Queenstown, River Valley, Sembawang, Sengkang) to Household Income to make a total of 30 Planning Areas
</commit_message>
<xml_diff>
--- a/Data/Household Income.xlsx
+++ b/Data/Household Income.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6F8ED85-1F38-4FED-8393-09E4209EE841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B12CE9E-C1F1-4DE6-B4F4-178C26F2E12C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="760" yWindow="320" windowWidth="17230" windowHeight="9880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="17578" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="194">
   <si>
     <t>Planning Area of Residence</t>
   </si>
@@ -585,13 +585,25 @@
   </si>
   <si>
     <t>Bukit Panjang</t>
+  </si>
+  <si>
+    <t>Queenstown</t>
+  </si>
+  <si>
+    <t>Sembawang</t>
+  </si>
+  <si>
+    <t>Sengkang</t>
+  </si>
+  <si>
+    <t>River Valley</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -603,6 +615,24 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -656,10 +686,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -679,9 +718,19 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="Hyperlink 2" xfId="6" xr:uid="{C8A72B97-9B0D-4292-B2D0-C32ECF538A00}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{CC8CCE6F-35AB-469C-B4D2-94F42E6E000A}"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{380E76BD-5707-4D06-A548-5B38B6C9AB4F}"/>
+    <cellStyle name="Normal 3 2" xfId="5" xr:uid="{C437BA1B-F2F5-460A-BA9B-5B0B3A6B7745}"/>
+    <cellStyle name="Normal 4" xfId="3" xr:uid="{9CC86206-8985-4D95-947D-F583071985F4}"/>
+    <cellStyle name="Normal 5" xfId="4" xr:uid="{C9C89F4D-D21B-4F5F-B68C-59DFCF675249}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1018,10 +1067,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U29"/>
+  <dimension ref="A1:U33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="116" zoomScaleNormal="116" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2460,457 +2509,717 @@
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A23" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="B23" s="4">
-        <v>38086</v>
-      </c>
-      <c r="C23" s="4">
-        <v>5318</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="E23" s="4">
-        <v>1444</v>
-      </c>
-      <c r="F23" s="4">
-        <v>1629</v>
-      </c>
-      <c r="G23" s="4">
-        <v>1464</v>
-      </c>
-      <c r="H23" s="3">
-        <v>1425</v>
-      </c>
-      <c r="I23" s="3">
-        <v>1786</v>
-      </c>
-      <c r="J23" s="3">
-        <v>1568</v>
-      </c>
-      <c r="K23" s="3">
-        <v>1803</v>
-      </c>
-      <c r="L23" s="3">
-        <v>1521</v>
-      </c>
-      <c r="M23" s="3">
-        <v>1470</v>
-      </c>
-      <c r="N23" s="3">
-        <v>1379</v>
-      </c>
-      <c r="O23" s="3">
-        <v>1255</v>
-      </c>
-      <c r="P23" s="3">
-        <v>1019</v>
-      </c>
-      <c r="Q23" s="3">
-        <v>1052</v>
-      </c>
-      <c r="R23" s="3">
-        <v>1008</v>
-      </c>
-      <c r="S23" s="3">
-        <v>2038</v>
-      </c>
-      <c r="T23" s="3">
-        <v>1795</v>
-      </c>
-      <c r="U23" s="3">
-        <v>8616</v>
+      <c r="A23" t="s">
+        <v>190</v>
+      </c>
+      <c r="B23" s="9">
+        <v>37053</v>
+      </c>
+      <c r="C23" s="9">
+        <v>7776</v>
+      </c>
+      <c r="D23" s="9">
+        <v>774</v>
+      </c>
+      <c r="E23" s="9">
+        <v>2408</v>
+      </c>
+      <c r="F23" s="9">
+        <v>1708</v>
+      </c>
+      <c r="G23" s="9">
+        <v>1924</v>
+      </c>
+      <c r="H23" s="9">
+        <v>1682</v>
+      </c>
+      <c r="I23" s="9">
+        <v>1515</v>
+      </c>
+      <c r="J23" s="9">
+        <v>1355</v>
+      </c>
+      <c r="K23" s="9">
+        <v>1304</v>
+      </c>
+      <c r="L23" s="9">
+        <v>1277</v>
+      </c>
+      <c r="M23" s="9">
+        <v>1264</v>
+      </c>
+      <c r="N23" s="9">
+        <v>1143</v>
+      </c>
+      <c r="O23" s="9">
+        <v>916</v>
+      </c>
+      <c r="P23" s="9">
+        <v>1174</v>
+      </c>
+      <c r="Q23" s="9">
+        <v>933</v>
+      </c>
+      <c r="R23" s="9">
+        <v>787</v>
+      </c>
+      <c r="S23" s="9">
+        <v>2083</v>
+      </c>
+      <c r="T23" s="9">
+        <v>1571</v>
+      </c>
+      <c r="U23" s="9">
+        <v>5460</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A24" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="B24" s="4">
-        <v>83681</v>
-      </c>
-      <c r="C24" s="4">
-        <v>9631</v>
-      </c>
-      <c r="D24" s="4">
-        <v>1389</v>
-      </c>
-      <c r="E24" s="4">
-        <v>4043</v>
-      </c>
-      <c r="F24" s="4">
-        <v>3892</v>
-      </c>
-      <c r="G24" s="4">
-        <v>4610</v>
-      </c>
-      <c r="H24" s="3">
-        <v>4472</v>
-      </c>
-      <c r="I24" s="3">
-        <v>4592</v>
-      </c>
-      <c r="J24" s="3">
-        <v>4362</v>
-      </c>
-      <c r="K24" s="3">
-        <v>4646</v>
-      </c>
-      <c r="L24" s="3">
-        <v>3802</v>
-      </c>
-      <c r="M24" s="3">
-        <v>4038</v>
-      </c>
-      <c r="N24" s="3">
-        <v>3947</v>
-      </c>
-      <c r="O24" s="3">
-        <v>3380</v>
-      </c>
-      <c r="P24" s="3">
-        <v>2975</v>
-      </c>
-      <c r="Q24" s="3">
-        <v>2903</v>
-      </c>
-      <c r="R24" s="3">
-        <v>2311</v>
-      </c>
-      <c r="S24" s="3">
-        <v>5373</v>
-      </c>
-      <c r="T24" s="3">
-        <v>3672</v>
-      </c>
-      <c r="U24" s="3">
-        <v>9644</v>
+    <row r="24" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="B24" s="9">
+        <v>3976</v>
+      </c>
+      <c r="C24" s="9">
+        <v>574</v>
+      </c>
+      <c r="D24" s="9">
+        <v>27</v>
+      </c>
+      <c r="E24" s="9">
+        <v>80</v>
+      </c>
+      <c r="F24" s="9">
+        <v>75</v>
+      </c>
+      <c r="G24" s="9">
+        <v>102</v>
+      </c>
+      <c r="H24" s="9">
+        <v>54</v>
+      </c>
+      <c r="I24" s="9">
+        <v>80</v>
+      </c>
+      <c r="J24" s="9">
+        <v>90</v>
+      </c>
+      <c r="K24" s="9">
+        <v>92</v>
+      </c>
+      <c r="L24" s="9">
+        <v>87</v>
+      </c>
+      <c r="M24" s="9">
+        <v>75</v>
+      </c>
+      <c r="N24" s="9">
+        <v>74</v>
+      </c>
+      <c r="O24" s="9">
+        <v>92</v>
+      </c>
+      <c r="P24" s="9">
+        <v>79</v>
+      </c>
+      <c r="Q24" s="9">
+        <v>59</v>
+      </c>
+      <c r="R24" s="9">
+        <v>85</v>
+      </c>
+      <c r="S24" s="9">
+        <v>195</v>
+      </c>
+      <c r="T24" s="9">
+        <v>197</v>
+      </c>
+      <c r="U24" s="9">
+        <v>1860</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A25" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="B25" s="4">
-        <v>7938</v>
-      </c>
-      <c r="C25" s="4">
-        <v>1210</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="J25" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="K25" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="L25" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="M25" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="N25" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="O25" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="P25" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q25" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="R25" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="S25" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="T25" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="U25" s="3">
-        <v>3977</v>
+      <c r="A25" t="s">
+        <v>191</v>
+      </c>
+      <c r="B25" s="9">
+        <v>33049</v>
+      </c>
+      <c r="C25" s="9">
+        <v>2716</v>
+      </c>
+      <c r="D25" s="9">
+        <v>586</v>
+      </c>
+      <c r="E25" s="9">
+        <v>1395</v>
+      </c>
+      <c r="F25" s="9">
+        <v>1695</v>
+      </c>
+      <c r="G25" s="9">
+        <v>2066</v>
+      </c>
+      <c r="H25" s="9">
+        <v>1979</v>
+      </c>
+      <c r="I25" s="9">
+        <v>2090</v>
+      </c>
+      <c r="J25" s="9">
+        <v>1931</v>
+      </c>
+      <c r="K25" s="9">
+        <v>1925</v>
+      </c>
+      <c r="L25" s="9">
+        <v>1882</v>
+      </c>
+      <c r="M25" s="9">
+        <v>1783</v>
+      </c>
+      <c r="N25" s="9">
+        <v>1645</v>
+      </c>
+      <c r="O25" s="9">
+        <v>1397</v>
+      </c>
+      <c r="P25" s="9">
+        <v>1237</v>
+      </c>
+      <c r="Q25" s="9">
+        <v>1310</v>
+      </c>
+      <c r="R25" s="9">
+        <v>1190</v>
+      </c>
+      <c r="S25" s="9">
+        <v>1866</v>
+      </c>
+      <c r="T25" s="9">
+        <v>1511</v>
+      </c>
+      <c r="U25" s="9">
+        <v>2847</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A26" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="B26" s="4">
-        <v>46880</v>
-      </c>
-      <c r="C26" s="4">
-        <v>10015</v>
-      </c>
-      <c r="D26" s="4">
-        <v>1296</v>
-      </c>
-      <c r="E26" s="4">
-        <v>2987</v>
-      </c>
-      <c r="F26" s="4">
-        <v>2376</v>
-      </c>
-      <c r="G26" s="4">
-        <v>2603</v>
-      </c>
-      <c r="H26" s="3">
-        <v>2504</v>
-      </c>
-      <c r="I26" s="3">
-        <v>2089</v>
-      </c>
-      <c r="J26" s="3">
-        <v>2072</v>
-      </c>
-      <c r="K26" s="3">
-        <v>1791</v>
-      </c>
-      <c r="L26" s="3">
-        <v>2004</v>
-      </c>
-      <c r="M26" s="3">
-        <v>1413</v>
-      </c>
-      <c r="N26" s="3">
-        <v>1484</v>
-      </c>
-      <c r="O26" s="3">
-        <v>1400</v>
-      </c>
-      <c r="P26" s="3">
-        <v>1202</v>
-      </c>
-      <c r="Q26" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="R26" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="S26" s="3">
-        <v>2236</v>
-      </c>
-      <c r="T26" s="3">
-        <v>1569</v>
-      </c>
-      <c r="U26" s="3">
-        <v>6064</v>
+      <c r="A26" t="s">
+        <v>192</v>
+      </c>
+      <c r="B26" s="9">
+        <v>79376</v>
+      </c>
+      <c r="C26" s="9">
+        <v>5621</v>
+      </c>
+      <c r="D26" s="9">
+        <v>1276</v>
+      </c>
+      <c r="E26" s="9">
+        <v>3166</v>
+      </c>
+      <c r="F26" s="9">
+        <v>3556</v>
+      </c>
+      <c r="G26" s="9">
+        <v>4024</v>
+      </c>
+      <c r="H26" s="9">
+        <v>4310</v>
+      </c>
+      <c r="I26" s="9">
+        <v>4318</v>
+      </c>
+      <c r="J26" s="9">
+        <v>4693</v>
+      </c>
+      <c r="K26" s="9">
+        <v>4431</v>
+      </c>
+      <c r="L26" s="9">
+        <v>4164</v>
+      </c>
+      <c r="M26" s="9">
+        <v>4359</v>
+      </c>
+      <c r="N26" s="9">
+        <v>3915</v>
+      </c>
+      <c r="O26" s="9">
+        <v>3803</v>
+      </c>
+      <c r="P26" s="9">
+        <v>3016</v>
+      </c>
+      <c r="Q26" s="9">
+        <v>3177</v>
+      </c>
+      <c r="R26" s="9">
+        <v>2811</v>
+      </c>
+      <c r="S26" s="9">
+        <v>6068</v>
+      </c>
+      <c r="T26" s="9">
+        <v>3905</v>
+      </c>
+      <c r="U26" s="9">
+        <v>8762</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="B27" s="4">
-        <v>78839</v>
+        <v>38086</v>
       </c>
       <c r="C27" s="4">
-        <v>7133</v>
-      </c>
-      <c r="D27" s="4">
-        <v>1293</v>
+        <v>5318</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>114</v>
       </c>
       <c r="E27" s="4">
-        <v>3913</v>
+        <v>1444</v>
       </c>
       <c r="F27" s="4">
-        <v>4488</v>
+        <v>1629</v>
       </c>
       <c r="G27" s="4">
-        <v>5132</v>
+        <v>1464</v>
       </c>
       <c r="H27" s="3">
-        <v>5032</v>
+        <v>1425</v>
       </c>
       <c r="I27" s="3">
-        <v>5584</v>
+        <v>1786</v>
       </c>
       <c r="J27" s="3">
-        <v>5249</v>
+        <v>1568</v>
       </c>
       <c r="K27" s="3">
-        <v>5025</v>
+        <v>1803</v>
       </c>
       <c r="L27" s="3">
-        <v>4606</v>
+        <v>1521</v>
       </c>
       <c r="M27" s="3">
-        <v>4596</v>
+        <v>1470</v>
       </c>
       <c r="N27" s="3">
-        <v>3379</v>
+        <v>1379</v>
       </c>
       <c r="O27" s="3">
-        <v>3239</v>
+        <v>1255</v>
       </c>
       <c r="P27" s="3">
-        <v>2861</v>
+        <v>1019</v>
       </c>
       <c r="Q27" s="3">
-        <v>2903</v>
+        <v>1052</v>
       </c>
       <c r="R27" s="3">
-        <v>2152</v>
+        <v>1008</v>
       </c>
       <c r="S27" s="3">
-        <v>4524</v>
+        <v>2038</v>
       </c>
       <c r="T27" s="3">
-        <v>2669</v>
+        <v>1795</v>
       </c>
       <c r="U27" s="3">
-        <v>5064</v>
+        <v>8616</v>
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="B28" s="4">
-        <v>75403</v>
+        <v>83681</v>
       </c>
       <c r="C28" s="4">
-        <v>8698</v>
+        <v>9631</v>
       </c>
       <c r="D28" s="4">
-        <v>1551</v>
+        <v>1389</v>
       </c>
       <c r="E28" s="4">
-        <v>4455</v>
+        <v>4043</v>
       </c>
       <c r="F28" s="4">
-        <v>4912</v>
+        <v>3892</v>
       </c>
       <c r="G28" s="4">
-        <v>4869</v>
+        <v>4610</v>
       </c>
       <c r="H28" s="3">
-        <v>4935</v>
+        <v>4472</v>
       </c>
       <c r="I28" s="3">
-        <v>5056</v>
+        <v>4592</v>
       </c>
       <c r="J28" s="3">
-        <v>4736</v>
+        <v>4362</v>
       </c>
       <c r="K28" s="3">
-        <v>4224</v>
+        <v>4646</v>
       </c>
       <c r="L28" s="3">
-        <v>3894</v>
+        <v>3802</v>
       </c>
       <c r="M28" s="3">
-        <v>3501</v>
+        <v>4038</v>
       </c>
       <c r="N28" s="3">
-        <v>3458</v>
+        <v>3947</v>
       </c>
       <c r="O28" s="3">
-        <v>3040</v>
+        <v>3380</v>
       </c>
       <c r="P28" s="3">
-        <v>2324</v>
+        <v>2975</v>
       </c>
       <c r="Q28" s="3">
-        <v>2349</v>
+        <v>2903</v>
       </c>
       <c r="R28" s="3">
-        <v>1883</v>
+        <v>2311</v>
       </c>
       <c r="S28" s="3">
-        <v>3689</v>
+        <v>5373</v>
       </c>
       <c r="T28" s="3">
-        <v>2429</v>
+        <v>3672</v>
       </c>
       <c r="U28" s="3">
-        <v>5399</v>
+        <v>9644</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B29" s="4">
+        <v>7938</v>
+      </c>
+      <c r="C29" s="4">
+        <v>1210</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="K29" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="L29" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="M29" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="N29" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="O29" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="P29" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q29" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="R29" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="S29" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="T29" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="U29" s="3">
+        <v>3977</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A30" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B30" s="4">
+        <v>46880</v>
+      </c>
+      <c r="C30" s="4">
+        <v>10015</v>
+      </c>
+      <c r="D30" s="4">
+        <v>1296</v>
+      </c>
+      <c r="E30" s="4">
+        <v>2987</v>
+      </c>
+      <c r="F30" s="4">
+        <v>2376</v>
+      </c>
+      <c r="G30" s="4">
+        <v>2603</v>
+      </c>
+      <c r="H30" s="3">
+        <v>2504</v>
+      </c>
+      <c r="I30" s="3">
+        <v>2089</v>
+      </c>
+      <c r="J30" s="3">
+        <v>2072</v>
+      </c>
+      <c r="K30" s="3">
+        <v>1791</v>
+      </c>
+      <c r="L30" s="3">
+        <v>2004</v>
+      </c>
+      <c r="M30" s="3">
+        <v>1413</v>
+      </c>
+      <c r="N30" s="3">
+        <v>1484</v>
+      </c>
+      <c r="O30" s="3">
+        <v>1400</v>
+      </c>
+      <c r="P30" s="3">
+        <v>1202</v>
+      </c>
+      <c r="Q30" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="R30" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S30" s="3">
+        <v>2236</v>
+      </c>
+      <c r="T30" s="3">
+        <v>1569</v>
+      </c>
+      <c r="U30" s="3">
+        <v>6064</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A31" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B31" s="4">
+        <v>78839</v>
+      </c>
+      <c r="C31" s="4">
+        <v>7133</v>
+      </c>
+      <c r="D31" s="4">
+        <v>1293</v>
+      </c>
+      <c r="E31" s="4">
+        <v>3913</v>
+      </c>
+      <c r="F31" s="4">
+        <v>4488</v>
+      </c>
+      <c r="G31" s="4">
+        <v>5132</v>
+      </c>
+      <c r="H31" s="3">
+        <v>5032</v>
+      </c>
+      <c r="I31" s="3">
+        <v>5584</v>
+      </c>
+      <c r="J31" s="3">
+        <v>5249</v>
+      </c>
+      <c r="K31" s="3">
+        <v>5025</v>
+      </c>
+      <c r="L31" s="3">
+        <v>4606</v>
+      </c>
+      <c r="M31" s="3">
+        <v>4596</v>
+      </c>
+      <c r="N31" s="3">
+        <v>3379</v>
+      </c>
+      <c r="O31" s="3">
+        <v>3239</v>
+      </c>
+      <c r="P31" s="3">
+        <v>2861</v>
+      </c>
+      <c r="Q31" s="3">
+        <v>2903</v>
+      </c>
+      <c r="R31" s="3">
+        <v>2152</v>
+      </c>
+      <c r="S31" s="3">
+        <v>4524</v>
+      </c>
+      <c r="T31" s="3">
+        <v>2669</v>
+      </c>
+      <c r="U31" s="3">
+        <v>5064</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A32" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B32" s="4">
+        <v>75403</v>
+      </c>
+      <c r="C32" s="4">
+        <v>8698</v>
+      </c>
+      <c r="D32" s="4">
+        <v>1551</v>
+      </c>
+      <c r="E32" s="4">
+        <v>4455</v>
+      </c>
+      <c r="F32" s="4">
+        <v>4912</v>
+      </c>
+      <c r="G32" s="4">
+        <v>4869</v>
+      </c>
+      <c r="H32" s="3">
+        <v>4935</v>
+      </c>
+      <c r="I32" s="3">
+        <v>5056</v>
+      </c>
+      <c r="J32" s="3">
+        <v>4736</v>
+      </c>
+      <c r="K32" s="3">
+        <v>4224</v>
+      </c>
+      <c r="L32" s="3">
+        <v>3894</v>
+      </c>
+      <c r="M32" s="3">
+        <v>3501</v>
+      </c>
+      <c r="N32" s="3">
+        <v>3458</v>
+      </c>
+      <c r="O32" s="3">
+        <v>3040</v>
+      </c>
+      <c r="P32" s="3">
+        <v>2324</v>
+      </c>
+      <c r="Q32" s="3">
+        <v>2349</v>
+      </c>
+      <c r="R32" s="3">
+        <v>1883</v>
+      </c>
+      <c r="S32" s="3">
+        <v>3689</v>
+      </c>
+      <c r="T32" s="3">
+        <v>2429</v>
+      </c>
+      <c r="U32" s="3">
+        <v>5399</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A33" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="B29" s="4">
+      <c r="B33" s="4">
         <v>12233</v>
       </c>
-      <c r="C29" s="4">
+      <c r="C33" s="4">
         <v>1698</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D33" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E33" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="F29" s="4" t="s">
+      <c r="F33" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="G29" s="4" t="s">
+      <c r="G33" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="H29" s="3" t="s">
+      <c r="H33" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="I29" s="3" t="s">
+      <c r="I33" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="J29" s="3" t="s">
+      <c r="J33" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="K29" s="3" t="s">
+      <c r="K33" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="L29" s="3" t="s">
+      <c r="L33" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="M29" s="3" t="s">
+      <c r="M33" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="N29" s="3" t="s">
+      <c r="N33" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="O29" s="3" t="s">
+      <c r="O33" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="P29" s="3" t="s">
+      <c r="P33" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="Q29" s="3" t="s">
+      <c r="Q33" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="R29" s="3" t="s">
+      <c r="R33" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="S29" s="3" t="s">
+      <c r="S33" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="T29" s="3" t="s">
+      <c r="T33" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="U29" s="3">
+      <c r="U33" s="3">
         <v>3691</v>
       </c>
     </row>

</xml_diff>